<commit_message>
column and row design
</commit_message>
<xml_diff>
--- a/assets/sheet.xlsx
+++ b/assets/sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27719"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFEC66D1-A6E6-4B11-8CEF-658BC527C897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B424B2B5-8387-4CA6-8028-B5332C78D0AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="11">
   <si>
     <t>Nome</t>
   </si>
@@ -40,6 +40,30 @@
   </si>
   <si>
     <t>Gustavo</t>
+  </si>
+  <si>
+    <t>Sheml</t>
+  </si>
+  <si>
+    <t>11ad16sa1dsa</t>
+  </si>
+  <si>
+    <t>OI</t>
+  </si>
+  <si>
+    <t>555+5asdsad</t>
+  </si>
+  <si>
+    <t>dsadas6ddsa</t>
+  </si>
+  <si>
+    <t>dsadas</t>
+  </si>
+  <si>
+    <t>dasd</t>
+  </si>
+  <si>
+    <t>sadsad</t>
   </si>
 </sst>
 </file>
@@ -411,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A26" sqref="A26:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -462,6 +486,230 @@
         <v>557198182456</v>
       </c>
     </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>557198182456</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>